<commit_message>
Finished up on the test bench and .do file for brent kung
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G23-9263-350-1257.xlsx
+++ b/Documentation/ProjectLog-G23-9263-350-1257.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylo\OneDrive\Desktop\ENSC350\DP2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011004B8-9E20-4075-B2AD-36E91819ABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F802966-D439-4899-A531-23099F2BFC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="uphip+fyQmgTbQWVslgKndYGTCUT2nMCnU8pTyuiPxh9t3MkaNQeLeeV1eDZUH8uYM8JtsIZJzZApwnnbRUEcA==" workbookSaltValue="PVE5+bPUyqyV9jE5EaqSxw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="4" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Tentative completion of timing testbench, and scripts, fixed run issue in the FS script</t>
+  </si>
+  <si>
+    <t>Spent time modifying the testbench again, added the status flag to the testbench, report of worst case propagation delay, organized the wave window better and converted the values to hex when necessary, improved the transcript files</t>
+  </si>
+  <si>
+    <t>Further modification of testbench to supress delay output for functional, added extra reports for simulation results, set up github for easier collaboration</t>
   </si>
 </sst>
 </file>
@@ -8795,8 +8801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAC5635-BB81-4716-B442-28EF74567593}">
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9022,8 +9028,12 @@
     </row>
     <row r="12" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="31"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C12" s="21">
+        <v>45973</v>
+      </c>
       <c r="D12" s="19">
         <v>0.875</v>
       </c>
@@ -9041,8 +9051,12 @@
     </row>
     <row r="13" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="31"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C13" s="21">
+        <v>45973</v>
+      </c>
       <c r="D13" s="19">
         <v>0.90625</v>
       </c>
@@ -9060,8 +9074,12 @@
     </row>
     <row r="14" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="31"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="21"/>
+      <c r="B14" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C14" s="21">
+        <v>45973</v>
+      </c>
       <c r="D14" s="19">
         <v>0.94444444444444442</v>
       </c>
@@ -9079,28 +9097,48 @@
     </row>
     <row r="15" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="31"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C15" s="21">
+        <v>45976</v>
+      </c>
+      <c r="D15" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.53125</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="H15" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.7500000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="31"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
+      <c r="B16" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C16" s="21">
+        <v>45976</v>
+      </c>
+      <c r="D16" s="19">
+        <v>0.53125</v>
+      </c>
+      <c r="E16" s="22">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2500000000000009</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.45">
@@ -9926,7 +9964,7 @@
       <c r="F80" s="29"/>
       <c r="H80" s="28">
         <f>SUM(H7:H79)</f>
-        <v>7.8666666666666663</v>
+        <v>10.866666666666667</v>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed the config stuff
</commit_message>
<xml_diff>
--- a/Documentation/ProjectLog-G23-9263-350-1257.xlsx
+++ b/Documentation/ProjectLog-G23-9263-350-1257.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylo\OneDrive\Desktop\ENSC350\DP2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F802966-D439-4899-A531-23099F2BFC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC320F-1418-4C40-9D4F-3CC3FA0E9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="uphip+fyQmgTbQWVslgKndYGTCUT2nMCnU8pTyuiPxh9t3MkaNQeLeeV1eDZUH8uYM8JtsIZJzZApwnnbRUEcA==" workbookSaltValue="PVE5+bPUyqyV9jE5EaqSxw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="4" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -484,6 +484,15 @@
   </si>
   <si>
     <t>Further modification of testbench to supress delay output for functional, added extra reports for simulation results, set up github for easier collaboration</t>
+  </si>
+  <si>
+    <t>Spent time experimenting and modifying the brent kung, tried not using components and using if statement levels to generate instead, found original still worked better</t>
+  </si>
+  <si>
+    <t>Spent time trying to change Brent Kung to reduce fanout to see if it improved performance, but it utilized 5 times the amount of LE's decided original was better</t>
+  </si>
+  <si>
+    <t>Split the config files up, because I realized that the work folder would delete every time and only compile the ones needed for the adder, but the config needed all the adders compiled, do I made multiple config files. Also finished some of the .do files</t>
   </si>
 </sst>
 </file>
@@ -8801,8 +8810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAC5635-BB81-4716-B442-28EF74567593}">
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9143,41 +9152,71 @@
     </row>
     <row r="17" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="31"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
+      <c r="B17" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C17" s="21">
+        <v>45976</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="H17" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="31"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="22"/>
+      <c r="B18" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C18" s="21">
+        <v>45976</v>
+      </c>
+      <c r="D18" s="19">
+        <v>0.8125</v>
+      </c>
+      <c r="E18" s="22">
+        <v>0.875</v>
+      </c>
       <c r="F18" s="34"/>
-      <c r="G18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="H18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="31"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="22"/>
+      <c r="B19" s="13">
+        <v>9263</v>
+      </c>
+      <c r="C19" s="21">
+        <v>45977</v>
+      </c>
+      <c r="D19" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="22">
+        <v>0.5625</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="16"/>
+      <c r="G19" s="16" t="s">
+        <v>46</v>
+      </c>
       <c r="H19" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.45">
@@ -9964,7 +10003,7 @@
       <c r="F80" s="29"/>
       <c r="H80" s="28">
         <f>SUM(H7:H79)</f>
-        <v>10.866666666666667</v>
+        <v>15.866666666666665</v>
       </c>
     </row>
     <row r="81" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>